<commit_message>
10 ish seconds to open app
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>company</t>
   </si>
@@ -25,13 +25,28 @@
     <t>active</t>
   </si>
   <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>sgrhdtjgf</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
+    <t>BC</t>
+  </si>
+  <si>
     <t>asset_type</t>
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>#562c33</t>
   </si>
   <si>
     <t>weight</t>
@@ -438,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -449,6 +464,22 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -457,15 +488,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -476,18 +515,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -503,7 +553,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -522,10 +572,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -541,25 +591,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -575,10 +625,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testing exceljs loading speed
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>company</t>
   </si>
@@ -25,28 +25,19 @@
     <t>active</t>
   </si>
   <si>
-    <t>test123</t>
+    <t>jkugjyh</t>
   </si>
   <si>
     <t>TRUE</t>
   </si>
   <si>
-    <t>sgrhdtjgf</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
-    <t>BC</t>
-  </si>
-  <si>
     <t>asset_type</t>
   </si>
   <si>
     <t>color</t>
-  </si>
-  <si>
-    <t>#562c33</t>
   </si>
   <si>
     <t>weight</t>
@@ -453,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,14 +463,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -488,23 +471,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -515,29 +490,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -553,7 +517,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -572,10 +536,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -591,25 +555,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -625,10 +589,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug with the import (new .xlsx wasnt created, and also pin issue
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>company</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>TRUE</t>
+  </si>
+  <si>
+    <t>bgwrer</t>
   </si>
   <si>
     <t>location</t>
@@ -453,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -472,6 +475,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -480,12 +491,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -493,10 +504,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -512,24 +531,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -545,7 +564,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -564,10 +583,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -583,25 +602,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -617,10 +636,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
There seem to be two differernt map pins, and the filters is not working as it should
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>company</t>
   </si>
@@ -31,9 +31,6 @@
     <t>TRUE</t>
   </si>
   <si>
-    <t>bgwrer</t>
-  </si>
-  <si>
     <t>location</t>
   </si>
   <si>
@@ -49,7 +46,7 @@
     <t>Cableway</t>
   </si>
   <si>
-    <t>#086119</t>
+    <t>#213916</t>
   </si>
   <si>
     <t>weight</t>
@@ -456,7 +453,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,14 +472,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -491,12 +480,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -504,18 +493,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -531,24 +512,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +545,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -583,10 +564,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -602,25 +583,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -636,10 +617,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Specific Station Details Section
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>company</t>
   </si>
@@ -34,12 +34,21 @@
     <t>TRUE</t>
   </si>
   <si>
+    <t>WSC</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
     <t>BC</t>
   </si>
   <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>YT</t>
+  </si>
+  <si>
     <t>asset_type</t>
   </si>
   <si>
@@ -55,7 +64,13 @@
     <t>Weir</t>
   </si>
   <si>
-    <t>#eeff00</t>
+    <t>#ff0000</t>
+  </si>
+  <si>
+    <t>#3eead6</t>
+  </si>
+  <si>
+    <t>#c425c8</t>
   </si>
   <si>
     <t>weight</t>
@@ -462,7 +477,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -484,6 +499,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -492,7 +515,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100"/>
   </sheetViews>
@@ -500,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -508,10 +531,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -522,7 +561,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="C5" sqref="C5"/>
@@ -532,35 +571,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -579,7 +640,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -601,10 +662,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -623,25 +684,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -660,10 +721,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import sync not working
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>company</t>
   </si>
@@ -37,6 +37,9 @@
     <t>BC</t>
   </si>
   <si>
+    <t>AB</t>
+  </si>
+  <si>
     <t>asset_type</t>
   </si>
   <si>
@@ -46,7 +49,10 @@
     <t>Cableway</t>
   </si>
   <si>
-    <t>#fc5d37</t>
+    <t>#bc97a3</t>
+  </si>
+  <si>
+    <t>#2df207</t>
   </si>
   <si>
     <t>weight</t>
@@ -480,7 +486,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -499,6 +505,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -507,12 +521,12 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -521,12 +535,12 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -535,7 +549,21 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -551,7 +579,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -570,10 +598,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -589,25 +617,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -623,10 +651,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the importing error finally
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>company</t>
   </si>
@@ -27,13 +27,28 @@
     <t>active</t>
   </si>
   <si>
+    <t>NHS</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
+    <t>BC</t>
+  </si>
+  <si>
     <t>asset_type</t>
   </si>
   <si>
     <t>color</t>
+  </si>
+  <si>
+    <t>Cableway</t>
+  </si>
+  <si>
+    <t>#4e9686</t>
   </si>
   <si>
     <t>weight</t>
@@ -476,7 +491,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -487,53 +502,83 @@
         <v>1</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -544,7 +589,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -552,7 +597,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -563,15 +608,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -582,92 +627,92 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
 
@@ -678,30 +723,30 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Maybe fixed typing bug
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>company</t>
   </si>
@@ -33,6 +33,9 @@
     <t>TRUE</t>
   </si>
   <si>
+    <t>Test</t>
+  </si>
+  <si>
     <t>location</t>
   </si>
   <si>
@@ -48,7 +51,10 @@
     <t>Cableway</t>
   </si>
   <si>
-    <t>#4e9686</t>
+    <t>#cd197e</t>
+  </si>
+  <si>
+    <t>#196ce1</t>
   </si>
   <si>
     <t>weight</t>
@@ -111,10 +117,10 @@
     <t>applyStatusColorsOnMap</t>
   </si>
   <si>
+    <t>applyRepairColorsOnMap</t>
+  </si>
+  <si>
     <t>FALSE</t>
-  </si>
-  <si>
-    <t>applyRepairColorsOnMap</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -510,6 +516,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -518,12 +532,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -531,12 +545,20 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
@@ -545,36 +567,50 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -589,7 +625,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -608,10 +644,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -627,87 +663,87 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -723,26 +759,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Repairs backend is done
</commit_message>
<xml_diff>
--- a/data/lookups.xlsx
+++ b/data/lookups.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>company</t>
   </si>
@@ -42,12 +42,6 @@
     <t>BC</t>
   </si>
   <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>\\int.ec.gc.ca\shares\ECCC\PVM\GV1\WSCInfrastructure\Stations_Alberta</t>
-  </si>
-  <si>
     <t>asset_type</t>
   </si>
   <si>
@@ -57,13 +51,7 @@
     <t>Cableway</t>
   </si>
   <si>
-    <t>#6a3a31</t>
-  </si>
-  <si>
-    <t>\\Ecbcv6cwvfsp001.ncr.int.ec.gc.ca\msc$\401\WSCConstruction\Stations</t>
-  </si>
-  <si>
-    <t>#36d227</t>
+    <t>#ccf610</t>
   </si>
   <si>
     <t>weight</t>
@@ -533,7 +521,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -555,31 +543,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
@@ -588,15 +565,15 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -605,33 +582,88 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G1"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>14</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
@@ -641,122 +673,50 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B1" t="s">
         <v>22</v>
-      </c>
-      <c r="F1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -772,26 +732,26 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>